<commit_message>
vita zay ny login succesful
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITU\semestre6\evaluation\git\daybyday-java\daybyday-java\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8DA7E-344C-49B4-A98A-CD482D8C7C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -18,9 +24,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+  <si>
+    <t>Tâches</t>
+  </si>
+  <si>
+    <t>Durée</t>
+  </si>
+  <si>
+    <t>Détails</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Création route /login</t>
+  </si>
+  <si>
+    <t>Creation controller AuthController avec la fonction login ()</t>
+  </si>
+  <si>
+    <t>Framework</t>
+  </si>
+  <si>
+    <t>Laravel</t>
+  </si>
+  <si>
+    <t>Ajout de dépendance webflux dans pom.xml</t>
+  </si>
+  <si>
+    <t>Spring Boot</t>
+  </si>
+  <si>
+    <t>Création de LaravelAuthService.java pour relier avec laravel</t>
+  </si>
+  <si>
+    <t>Configurer l'url de l'api dans application-properties localhost:80000/api</t>
+  </si>
+  <si>
+    <t>Création de index.html dans lequel se trouve le login en utilisant Thymeleaf</t>
+  </si>
+  <si>
+    <t>Installer la bibliothèque Sanctum pour créer un token</t>
+  </si>
+  <si>
+    <t>Debug</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +84,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -49,8 +119,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +403,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
vita koa louni zay ny dashboard
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITU\semestre6\evaluation\git\daybyday-java\daybyday-java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C8DA7E-344C-49B4-A98A-CD482D8C7C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F01102-7DE9-4FC1-809E-3DEE04572874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Tâches</t>
   </si>
@@ -70,13 +70,40 @@
   </si>
   <si>
     <t>Debug</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>Creation DashboardController</t>
+  </si>
+  <si>
+    <t>Creation entity DashboardData qui regroupe les entités ci-dessous</t>
+  </si>
+  <si>
+    <t>Absence, Departement, Settings, User</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Creation de LaravelDashboardService avec la fonction</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> getDashboardData qui vise Laravel en utilisant RestTemplate</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>affichage dashboard:ht,l</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,8 +119,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +136,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -119,10 +164,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -404,20 +457,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" customWidth="1"/>
+    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,110 +483,200 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="2"/>
+      <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="3">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="2"/>
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="2"/>
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
+      <c r="D6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="3">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="2"/>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9">
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="2"/>
+      <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="C11" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="2"/>
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3">
         <v>120</v>
       </c>
     </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="4">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:B11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>